<commit_message>
Completed build of App with documentation and help.
</commit_message>
<xml_diff>
--- a/app/example/Sample_add_vars.xlsx
+++ b/app/example/Sample_add_vars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Code\muiModels\TableViewer\app\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC770494-3443-4C03-A114-73291E547FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F07A21-6784-41A2-BF8E-6309958A4B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="3340" windowWidth="28800" windowHeight="15370" xr2:uid="{F4AAEDD5-7F93-40DE-AD60-EA840305CCC7}"/>
+    <workbookView xWindow="50440" yWindow="4560" windowWidth="28800" windowHeight="15370" xr2:uid="{F4AAEDD5-7F93-40DE-AD60-EA840305CCC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Hmhw</t>
   </si>
@@ -45,6 +45,42 @@
   </si>
   <si>
     <t>Hmlw</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Hayle Estuary</t>
+  </si>
+  <si>
+    <t>Gannel Estuary</t>
+  </si>
+  <si>
+    <t>Camel Estuary</t>
+  </si>
+  <si>
+    <t>Bridgwater Bay</t>
+  </si>
+  <si>
+    <t>Severn Estuary</t>
+  </si>
+  <si>
+    <t>Axe Estuary</t>
+  </si>
+  <si>
+    <t>Otter Estuary</t>
+  </si>
+  <si>
+    <t>Exe Estuary</t>
+  </si>
+  <si>
+    <t>Teign Estuary</t>
+  </si>
+  <si>
+    <t>Dart Estuary</t>
+  </si>
+  <si>
+    <t>Salcombe &amp; Kingsbridge Estuary</t>
   </si>
 </sst>
 </file>
@@ -400,143 +436,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046DB27E-65BA-4A1F-AD76-BA835FAD5C42}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
         <v>2.5945477590820385</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>18.138109118982019</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>16.069336471565538</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
         <v>2.6007805710386314</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1">
         <v>5.0278214742332814</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>2.8271043496454937</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
         <v>4.6442439823656851</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="1">
         <v>4.5542310462498845</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>4.5509584694617597</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
         <v>4.3084554248826956</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
         <v>3.4238383107056145</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>0.35342603388645066</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
         <v>11.571311126048059</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6" s="1">
         <v>9.481181257127977</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>5.5095583550507792</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
         <v>0.62011173184357538</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7" s="1">
         <v>0.4351598173515982</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>0.1673704414587332</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
         <v>1.7785714285714285</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C8" s="1">
         <v>1.2589285714285714</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>0.57796257796257799</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
         <v>2.5911602209944751</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C9" s="1">
         <v>2.1226415094339623</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>0.70107238605898126</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1">
         <v>2.6858638743455496</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>2.407766990291262</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>3.2123287671232879</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
         <v>4.8039215686274508</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C11" s="1">
         <v>5.1791044776119399</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>3.484320557491289</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
         <v>1.4</v>
       </c>
-      <c r="B12" s="1">
+      <c r="C12" s="1">
         <v>2.4729241877256318</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>1.3172413793103448</v>
       </c>
     </row>

</xml_diff>